<commit_message>
feat(api): add api endpoint spanish league
</commit_message>
<xml_diff>
--- a/src/template.xlsx
+++ b/src/template.xlsx
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t xml:space="preserve">Jornada X</t>
-  </si>
-  <si>
     <t xml:space="preserve">Encuentros</t>
   </si>
   <si>
@@ -37,19 +34,22 @@
     <t xml:space="preserve">Visitante</t>
   </si>
   <si>
-    <t xml:space="preserve">Persona 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Persona 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Persona 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Persona 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Persona 5</t>
+    <t xml:space="preserve">Joan Casals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David Casals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lluís Codina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nacho Do-cal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eduardo Poch </t>
+  </si>
+  <si>
+    <t xml:space="preserve">David Serra</t>
   </si>
 </sst>
 </file>
@@ -91,7 +91,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="0"/>
@@ -147,28 +147,32 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -361,204 +365,246 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="25.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="25.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="36.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="25.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="24.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="25.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="25.18"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2"/>
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:H1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>